<commit_message>
correcting units, refactoring rate law calculations, other debugging
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_broken_kb.xlsx
+++ b/tests/fixtures/test_broken_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" activeTab="3"/>
+    <workbookView windowWidth="28695" windowHeight="13965" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Gene loci'!$A$1:$J$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Protein species types'!$A$1:$I$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$K$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Concentrations!$A$1:$E$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Concentrations!$A$1:$E$97</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Reactions!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Rate laws'!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Properties!$A$1:$F$5</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="530">
   <si>
     <t>Id</t>
   </si>
@@ -1222,6 +1222,9 @@
     <t>cmp[c]</t>
   </si>
   <si>
+    <t>cdp[c]</t>
+  </si>
+  <si>
     <t>ctp[c]</t>
   </si>
   <si>
@@ -1474,6 +1477,9 @@
     <t>ump[c]</t>
   </si>
   <si>
+    <t>udp[c]</t>
+  </si>
+  <si>
     <t>utp[c]</t>
   </si>
   <si>
@@ -1522,22 +1528,22 @@
     <t>forward</t>
   </si>
   <si>
-    <t>0.000000007312742167607660744</t>
+    <t>k_cat_conv</t>
   </si>
   <si>
     <t>mock_transfer_2amp_forward</t>
   </si>
   <si>
-    <t>0.001*k_cat+k_m</t>
+    <t>k_cat_transfer</t>
   </si>
   <si>
     <t>Error</t>
   </si>
   <si>
-    <t>k_cat</t>
-  </si>
-  <si>
-    <t>k_m</t>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>K_m</t>
   </si>
   <si>
     <t>mean_doubling_time</t>
@@ -1838,7 +1844,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1861,12 +1867,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -2165,103 +2165,103 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2276,7 +2276,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2297,10 +2297,10 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2310,7 +2310,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2320,9 +2320,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3710,18 +3707,19 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
+    <col min="2" max="2" width="9.375"/>
     <col min="6" max="6" width="18.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3854,7 +3852,7 @@
         <v>390</v>
       </c>
       <c r="B10" s="2">
-        <v>0.0012</v>
+        <v>0.001</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>382</v>
@@ -3867,7 +3865,7 @@
         <v>391</v>
       </c>
       <c r="B11" s="2">
-        <v>0.00037</v>
+        <v>0.0012</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>382</v>
@@ -3880,7 +3878,7 @@
         <v>392</v>
       </c>
       <c r="B12" s="2">
-        <v>0.005</v>
+        <v>0.00037</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>382</v>
@@ -3893,7 +3891,7 @@
         <v>393</v>
       </c>
       <c r="B13" s="2">
-        <v>0.0038</v>
+        <v>0.005</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>382</v>
@@ -3906,7 +3904,7 @@
         <v>394</v>
       </c>
       <c r="B14" s="2">
-        <v>0.096</v>
+        <v>0.0038</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>382</v>
@@ -3919,7 +3917,7 @@
         <v>395</v>
       </c>
       <c r="B15" s="2">
-        <v>0.0031</v>
+        <v>0.096</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>382</v>
@@ -3932,7 +3930,7 @@
         <v>396</v>
       </c>
       <c r="B16" s="2">
-        <v>2.4e-5</v>
+        <v>0.0031</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>382</v>
@@ -3945,7 +3943,7 @@
         <v>397</v>
       </c>
       <c r="B17" s="2">
-        <v>0.0019</v>
+        <v>2.4e-5</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>382</v>
@@ -3958,7 +3956,7 @@
         <v>398</v>
       </c>
       <c r="B18" s="2">
-        <v>55.5</v>
+        <v>0.0019</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>382</v>
@@ -3971,7 +3969,7 @@
         <v>399</v>
       </c>
       <c r="B19" s="2">
-        <v>2.82e-8</v>
+        <v>55.5</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>382</v>
@@ -3984,7 +3982,7 @@
         <v>400</v>
       </c>
       <c r="B20" s="2">
-        <v>6.8e-5</v>
+        <v>2.82e-8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>382</v>
@@ -3997,7 +3995,7 @@
         <v>401</v>
       </c>
       <c r="B21" s="2">
-        <v>0.0003</v>
+        <v>6.8e-5</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>382</v>
@@ -4023,7 +4021,7 @@
         <v>403</v>
       </c>
       <c r="B23" s="2">
-        <v>0.00041</v>
+        <v>0.0003</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>382</v>
@@ -4036,7 +4034,7 @@
         <v>404</v>
       </c>
       <c r="B24" s="2">
-        <v>0.00015</v>
+        <v>0.00041</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>382</v>
@@ -4049,7 +4047,7 @@
         <v>405</v>
       </c>
       <c r="B25" s="2">
-        <v>1.8e-5</v>
+        <v>0.00015</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>382</v>
@@ -4062,7 +4060,7 @@
         <v>406</v>
       </c>
       <c r="B26" s="2">
-        <v>0.005</v>
+        <v>1.8e-5</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>382</v>
@@ -4075,7 +4073,7 @@
         <v>407</v>
       </c>
       <c r="B27" s="2">
-        <v>0.0005</v>
+        <v>0.005</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>382</v>
@@ -4088,7 +4086,7 @@
         <v>408</v>
       </c>
       <c r="B28" s="2">
-        <v>0.00039</v>
+        <v>0.0005</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>382</v>
@@ -4101,7 +4099,7 @@
         <v>409</v>
       </c>
       <c r="B29" s="2">
-        <v>1.69042874315485e-6</v>
+        <v>0.00039</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>382</v>
@@ -4114,7 +4112,7 @@
         <v>410</v>
       </c>
       <c r="B30" s="2">
-        <v>1.67050227466973e-6</v>
+        <v>1.69042874315485e-6</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>382</v>
@@ -4127,7 +4125,7 @@
         <v>411</v>
       </c>
       <c r="B31" s="2">
-        <v>1.68212604795272e-6</v>
+        <v>1.67050227466973e-6</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>382</v>
@@ -4140,7 +4138,7 @@
         <v>412</v>
       </c>
       <c r="B32" s="2">
-        <v>1.71035521163998e-6</v>
+        <v>1.68212604795272e-6</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>382</v>
@@ -4153,7 +4151,7 @@
         <v>413</v>
       </c>
       <c r="B33" s="2">
-        <v>1.67050227466973e-6</v>
+        <v>1.71035521163998e-6</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>382</v>
@@ -4166,7 +4164,7 @@
         <v>414</v>
       </c>
       <c r="B34" s="2">
-        <v>1.64891526714417e-6</v>
+        <v>1.67050227466973e-6</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>382</v>
@@ -4179,7 +4177,7 @@
         <v>415</v>
       </c>
       <c r="B35" s="2">
-        <v>1.67880496987186e-6</v>
+        <v>1.64891526714417e-6</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>382</v>
@@ -4192,7 +4190,7 @@
         <v>416</v>
       </c>
       <c r="B36" s="2">
-        <v>1.68212604795272e-6</v>
+        <v>1.67880496987186e-6</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>382</v>
@@ -4205,7 +4203,7 @@
         <v>417</v>
       </c>
       <c r="B37" s="2">
-        <v>1.67050227466973e-6</v>
+        <v>1.68212604795272e-6</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>382</v>
@@ -4218,7 +4216,7 @@
         <v>418</v>
       </c>
       <c r="B38" s="2">
-        <v>1.63895203290161e-6</v>
+        <v>1.67050227466973e-6</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>382</v>
@@ -4231,7 +4229,7 @@
         <v>419</v>
       </c>
       <c r="B39" s="2">
-        <v>1.6688417356293e-6</v>
+        <v>1.63895203290161e-6</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>382</v>
@@ -4244,7 +4242,7 @@
         <v>420</v>
       </c>
       <c r="B40" s="2">
-        <v>1.66219957946759e-6</v>
+        <v>1.6688417356293e-6</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>382</v>
@@ -4270,7 +4268,7 @@
         <v>422</v>
       </c>
       <c r="B42" s="2">
-        <v>1.65721796234631e-6</v>
+        <v>1.66219957946759e-6</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>382</v>
@@ -4283,7 +4281,7 @@
         <v>423</v>
       </c>
       <c r="B43" s="2">
-        <v>1.73194221916553e-6</v>
+        <v>1.65721796234631e-6</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>382</v>
@@ -4296,7 +4294,7 @@
         <v>424</v>
       </c>
       <c r="B44" s="2">
-        <v>1.66053904042716e-6</v>
+        <v>1.73194221916553e-6</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>382</v>
@@ -4309,7 +4307,7 @@
         <v>425</v>
       </c>
       <c r="B45" s="2">
-        <v>1.65389688426545e-6</v>
+        <v>1.66053904042716e-6</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>382</v>
@@ -4322,7 +4320,7 @@
         <v>426</v>
       </c>
       <c r="B46" s="2">
-        <v>1.62732825961862e-6</v>
+        <v>1.65389688426545e-6</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>382</v>
@@ -4335,7 +4333,7 @@
         <v>427</v>
       </c>
       <c r="B47" s="2">
-        <v>1.65223634522503e-6</v>
+        <v>1.62732825961862e-6</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>382</v>
@@ -4348,7 +4346,7 @@
         <v>428</v>
       </c>
       <c r="B48" s="2">
-        <v>1.65721796234631e-6</v>
+        <v>1.65223634522503e-6</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>382</v>
@@ -4361,7 +4359,7 @@
         <v>429</v>
       </c>
       <c r="B49" s="2">
-        <v>1.69208928219528e-6</v>
+        <v>1.65721796234631e-6</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>382</v>
@@ -4374,7 +4372,7 @@
         <v>430</v>
       </c>
       <c r="B50" s="2">
-        <v>1.6140439472952e-6</v>
+        <v>1.69208928219528e-6</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>382</v>
@@ -4387,7 +4385,7 @@
         <v>431</v>
       </c>
       <c r="B51" s="2">
-        <v>1.69541036027613e-6</v>
+        <v>1.6140439472952e-6</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>382</v>
@@ -4400,7 +4398,7 @@
         <v>432</v>
       </c>
       <c r="B52" s="2">
-        <v>1.64559418906332e-6</v>
+        <v>1.69541036027613e-6</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>382</v>
@@ -4413,7 +4411,7 @@
         <v>433</v>
       </c>
       <c r="B53" s="2">
-        <v>1.70205251643784e-6</v>
+        <v>1.64559418906332e-6</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>382</v>
@@ -4426,7 +4424,7 @@
         <v>434</v>
       </c>
       <c r="B54" s="2">
-        <v>1.65721796234631e-6</v>
+        <v>1.70205251643784e-6</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>382</v>
@@ -4439,7 +4437,7 @@
         <v>435</v>
       </c>
       <c r="B55" s="2">
-        <v>1.63064933769947e-6</v>
+        <v>1.65721796234631e-6</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>382</v>
@@ -4452,7 +4450,7 @@
         <v>436</v>
       </c>
       <c r="B56" s="2">
-        <v>1.64559418906332e-6</v>
+        <v>1.63064933769947e-6</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>382</v>
@@ -4465,7 +4463,7 @@
         <v>437</v>
       </c>
       <c r="B57" s="2">
-        <v>1.66053904042716e-6</v>
+        <v>1.64559418906332e-6</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>382</v>
@@ -4478,7 +4476,7 @@
         <v>438</v>
       </c>
       <c r="B58" s="2">
-        <v>1.66718119658887e-6</v>
+        <v>1.66053904042716e-6</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>382</v>
@@ -4491,7 +4489,7 @@
         <v>439</v>
       </c>
       <c r="B59" s="2">
-        <v>1.68544712603357e-6</v>
+        <v>1.66718119658887e-6</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>382</v>
@@ -4504,7 +4502,7 @@
         <v>440</v>
       </c>
       <c r="B60" s="2">
-        <v>1.67880496987186e-6</v>
+        <v>1.68544712603357e-6</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>382</v>
@@ -4517,7 +4515,7 @@
         <v>441</v>
       </c>
       <c r="B61" s="2">
-        <v>1.66053904042716e-7</v>
+        <v>1.67880496987186e-6</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>382</v>
@@ -4530,7 +4528,7 @@
         <v>442</v>
       </c>
       <c r="B62" s="2">
-        <v>1.89301450608697e-7</v>
+        <v>1.66053904042716e-7</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>382</v>
@@ -4543,7 +4541,7 @@
         <v>443</v>
       </c>
       <c r="B63" s="2">
-        <v>1.41145818436309e-7</v>
+        <v>1.89301450608697e-7</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>382</v>
@@ -4556,7 +4554,7 @@
         <v>444</v>
       </c>
       <c r="B64" s="2">
-        <v>1.92622528689551e-7</v>
+        <v>1.41145818436309e-7</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>382</v>
@@ -4569,7 +4567,7 @@
         <v>445</v>
       </c>
       <c r="B65" s="2">
-        <v>1.85980372527842e-7</v>
+        <v>1.92622528689551e-7</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>382</v>
@@ -4582,7 +4580,7 @@
         <v>446</v>
       </c>
       <c r="B66" s="2">
-        <v>1.31182584193746e-7</v>
+        <v>1.85980372527842e-7</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>382</v>
@@ -4595,7 +4593,7 @@
         <v>447</v>
       </c>
       <c r="B67" s="2">
-        <v>1.62732825961862e-7</v>
+        <v>1.31182584193746e-7</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>382</v>
@@ -4608,7 +4606,7 @@
         <v>448</v>
       </c>
       <c r="B68" s="2">
-        <v>2.09227919093823e-7</v>
+        <v>1.62732825961862e-7</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>382</v>
@@ -4621,7 +4619,7 @@
         <v>449</v>
       </c>
       <c r="B69" s="2">
-        <v>1.71035521163998e-7</v>
+        <v>2.09227919093823e-7</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>382</v>
@@ -4634,7 +4632,7 @@
         <v>450</v>
       </c>
       <c r="B70" s="2">
-        <v>1.52769591719299e-7</v>
+        <v>1.71035521163998e-7</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>382</v>
@@ -4647,7 +4645,7 @@
         <v>451</v>
       </c>
       <c r="B71" s="2">
-        <v>1.54430130759726e-7</v>
+        <v>1.52769591719299e-7</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>382</v>
@@ -4660,7 +4658,7 @@
         <v>452</v>
       </c>
       <c r="B72" s="2">
-        <v>1.59411747881008e-7</v>
+        <v>1.54430130759726e-7</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>382</v>
@@ -4673,7 +4671,7 @@
         <v>453</v>
       </c>
       <c r="B73" s="2">
-        <v>1.85980372527842e-7</v>
+        <v>1.59411747881008e-7</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>382</v>
@@ -4686,7 +4684,7 @@
         <v>454</v>
       </c>
       <c r="B74" s="2">
-        <v>1.71035521163998e-7</v>
+        <v>1.85980372527842e-7</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>382</v>
@@ -4699,7 +4697,7 @@
         <v>455</v>
       </c>
       <c r="B75" s="2">
-        <v>1.80998755406561e-7</v>
+        <v>1.71035521163998e-7</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>382</v>
@@ -4712,7 +4710,7 @@
         <v>456</v>
       </c>
       <c r="B76" s="2">
-        <v>1.9926468485126e-7</v>
+        <v>1.80998755406561e-7</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>382</v>
@@ -4725,7 +4723,7 @@
         <v>457</v>
       </c>
       <c r="B77" s="2">
-        <v>1.42806357476736e-7</v>
+        <v>1.9926468485126e-7</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>382</v>
@@ -4738,7 +4736,7 @@
         <v>458</v>
       </c>
       <c r="B78" s="2">
-        <v>1.76017138285279e-7</v>
+        <v>1.42806357476736e-7</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>382</v>
@@ -4751,7 +4749,7 @@
         <v>459</v>
       </c>
       <c r="B79" s="2">
-        <v>1.82659294446988e-7</v>
+        <v>1.76017138285279e-7</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>382</v>
@@ -4764,7 +4762,7 @@
         <v>460</v>
       </c>
       <c r="B80" s="2">
-        <v>1.90961989649124e-7</v>
+        <v>1.82659294446988e-7</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>382</v>
@@ -4777,7 +4775,7 @@
         <v>461</v>
       </c>
       <c r="B81" s="2">
-        <v>1.69374982123571e-7</v>
+        <v>1.90961989649124e-7</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>382</v>
@@ -4790,7 +4788,7 @@
         <v>462</v>
       </c>
       <c r="B82" s="2">
-        <v>1.54430130759726e-7</v>
+        <v>1.69374982123571e-7</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>382</v>
@@ -4803,7 +4801,7 @@
         <v>463</v>
       </c>
       <c r="B83" s="2">
-        <v>1.72696060204425e-7</v>
+        <v>1.54430130759726e-7</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>382</v>
@@ -4816,7 +4814,7 @@
         <v>464</v>
       </c>
       <c r="B84" s="2">
-        <v>1.71035521163998e-7</v>
+        <v>1.72696060204425e-7</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>382</v>
@@ -4829,7 +4827,7 @@
         <v>465</v>
       </c>
       <c r="B85" s="2">
-        <v>1.52769591719299e-7</v>
+        <v>1.71035521163998e-7</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>382</v>
@@ -4842,7 +4840,7 @@
         <v>466</v>
       </c>
       <c r="B86" s="2">
-        <v>1.77677677325707e-7</v>
+        <v>1.52769591719299e-7</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>382</v>
@@ -4855,7 +4853,7 @@
         <v>467</v>
       </c>
       <c r="B87" s="2">
-        <v>1.69374982123571e-7</v>
+        <v>1.77677677325707e-7</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>382</v>
@@ -4868,7 +4866,7 @@
         <v>468</v>
       </c>
       <c r="B88" s="2">
-        <v>1.54430130759726e-7</v>
+        <v>1.69374982123571e-7</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>382</v>
@@ -4881,7 +4879,7 @@
         <v>469</v>
       </c>
       <c r="B89" s="2">
-        <v>6.8e-5</v>
+        <v>1.54430130759726e-7</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>382</v>
@@ -4894,7 +4892,7 @@
         <v>470</v>
       </c>
       <c r="B90" s="2">
-        <v>0.00018</v>
+        <v>6.8e-5</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>382</v>
@@ -4907,7 +4905,7 @@
         <v>471</v>
       </c>
       <c r="B91" s="2">
-        <v>1.2e-5</v>
+        <v>0.00018</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>382</v>
@@ -4920,7 +4918,7 @@
         <v>472</v>
       </c>
       <c r="B92" s="2">
-        <v>2.9e-5</v>
+        <v>1.2e-5</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>382</v>
@@ -4933,7 +4931,7 @@
         <v>473</v>
       </c>
       <c r="B93" s="2">
-        <v>0.000184</v>
+        <v>2.9e-5</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>382</v>
@@ -4946,7 +4944,7 @@
         <v>474</v>
       </c>
       <c r="B94" s="2">
-        <v>0.002</v>
+        <v>0.000184</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>382</v>
@@ -4959,7 +4957,7 @@
         <v>475</v>
       </c>
       <c r="B95" s="2">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>382</v>
@@ -4967,8 +4965,34 @@
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
     </row>
+    <row r="96" ht="15" customHeight="1" spans="1:5">
+      <c r="A96" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.002</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" ht="15" customHeight="1" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.004</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E95">
+  <autoFilter ref="A1:E97">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4986,7 +5010,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -5007,13 +5031,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -5027,14 +5051,14 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>0</v>
@@ -5046,14 +5070,14 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -5082,7 +5106,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
@@ -5094,16 +5118,16 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>380</v>
@@ -5119,41 +5143,41 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>479</v>
+      <c r="A2" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C3" t="s">
         <v>491</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="C3" t="s">
-        <v>489</v>
-      </c>
       <c r="D3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G3">
@@ -5168,13 +5192,18 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
@@ -5186,13 +5215,13 @@
       <c r="C1" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>493</v>
+      <c r="D1" s="4" t="s">
+        <v>495</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -5202,20 +5231,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>494</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5e-5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C3">
+        <v>7.31274216760766e-9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C4">
         <v>0.075</v>
+      </c>
+      <c r="E4" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -5267,56 +5313,56 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <v>1000000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>1e-15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5356,7 +5402,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>380</v>
@@ -5373,13 +5419,13 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5389,13 +5435,13 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -5405,13 +5451,13 @@
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -5421,13 +5467,13 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>376</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -5437,13 +5483,13 @@
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -5453,13 +5499,13 @@
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -5469,13 +5515,13 @@
     </row>
     <row r="8" ht="15" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -5485,13 +5531,13 @@
     </row>
     <row r="9" ht="15" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -5501,13 +5547,13 @@
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -5517,13 +5563,13 @@
     </row>
     <row r="11" ht="15" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -5533,13 +5579,13 @@
     </row>
     <row r="12" ht="15" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -5549,13 +5595,13 @@
     </row>
     <row r="13" ht="15" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -5592,7 +5638,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -5729,7 +5775,7 @@
   <sheetPr/>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -7185,7 +7231,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
updating for renaming DatabaseReference-->Identifier, removing Author.orcid in wc-lang
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_broken_kb.xlsx
+++ b/tests/fixtures/test_broken_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" firstSheet="9" activeTab="11"/>
+    <workbookView windowWidth="20295" windowHeight="6840" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
     <t>References</t>
   </si>
   <si>
-    <t>Database References</t>
+    <t>Identifiers</t>
   </si>
   <si>
     <t>c</t>
@@ -1647,12 +1647,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1682,26 +1682,45 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1723,37 +1742,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1761,7 +1749,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1772,14 +1760,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1799,15 +1779,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1822,6 +1794,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1830,9 +1809,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1871,7 +1858,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1889,114 +2002,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2009,13 +2014,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2027,31 +2038,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2065,26 +2052,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2119,6 +2097,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2128,17 +2121,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2146,8 +2133,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2165,130 +2152,109 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2297,20 +2263,41 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2322,13 +2309,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3714,7 +3698,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -5143,10 +5127,10 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>481</v>
       </c>
       <c r="C2" t="s">
@@ -5160,10 +5144,10 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>484</v>
       </c>
       <c r="C3" t="s">
@@ -5177,7 +5161,7 @@
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="7"/>
+      <c r="B4" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G3">

</xml_diff>